<commit_message>
Trying to fix the housing stock rebuild process
</commit_message>
<xml_diff>
--- a/inputs/desaster_input_data_template.xlsx
+++ b/inputs/desaster_input_data_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="renters" sheetId="5" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="52">
   <si>
     <t>Savings</t>
   </si>
@@ -174,6 +174,18 @@
   </si>
   <si>
     <t>Extensive</t>
+  </si>
+  <si>
+    <t>Jerome</t>
+  </si>
+  <si>
+    <t>Barbara</t>
+  </si>
+  <si>
+    <t>Lucas</t>
+  </si>
+  <si>
+    <t>Dick</t>
   </si>
 </sst>
 </file>
@@ -714,7 +726,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection sqref="A1:L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -919,156 +931,201 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2">
+        <v>100000000</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>22</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2">
+        <v>1000</v>
+      </c>
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="C2">
-        <v>100</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
         <v>1100</v>
       </c>
-      <c r="G2">
+      <c r="J2">
         <v>1920</v>
       </c>
-      <c r="H2">
+      <c r="K2">
         <v>100000</v>
       </c>
-      <c r="I2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3">
+        <v>100000000</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
         <v>23</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E3">
+        <v>4000</v>
+      </c>
+      <c r="F3" t="s">
         <v>15</v>
       </c>
-      <c r="C3">
-        <v>100000</v>
-      </c>
-      <c r="D3">
+      <c r="G3">
         <v>4</v>
       </c>
-      <c r="E3">
+      <c r="H3">
         <v>5</v>
       </c>
-      <c r="F3">
+      <c r="I3">
         <v>5000</v>
       </c>
-      <c r="G3">
+      <c r="J3">
         <v>1920</v>
       </c>
-      <c r="H3">
+      <c r="K3">
         <v>10000000</v>
       </c>
-      <c r="I3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4">
+        <v>100000000</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
         <v>24</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4">
+        <v>1000</v>
+      </c>
+      <c r="F4" t="s">
         <v>15</v>
       </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
         <v>1200</v>
       </c>
-      <c r="G4">
+      <c r="J4">
         <v>1960</v>
       </c>
-      <c r="H4">
+      <c r="K4">
         <v>10000</v>
       </c>
-      <c r="I4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5">
+        <v>100000000</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
         <v>25</v>
       </c>
-      <c r="B5" t="s">
+      <c r="E5">
+        <v>2000</v>
+      </c>
+      <c r="F5" t="s">
         <v>15</v>
       </c>
-      <c r="C5">
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
         <v>2000</v>
       </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5">
-        <v>2000</v>
-      </c>
-      <c r="G5">
+      <c r="J5">
         <v>2010</v>
       </c>
-      <c r="H5">
+      <c r="K5">
         <v>800000</v>
       </c>
-      <c r="I5" t="s">
+      <c r="L5" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1081,8 +1138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Finally fixed process for repairing vacant building stocks; created importEntities to replace importOwnerHouseholds etc.
</commit_message>
<xml_diff>
--- a/inputs/desaster_input_data_template.xlsx
+++ b/inputs/desaster_input_data_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="renters" sheetId="5" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="55">
   <si>
     <t>Savings</t>
   </si>
@@ -86,9 +86,6 @@
     <t>1001 Other Ave</t>
   </si>
   <si>
-    <t>Multi Family Dwelling</t>
-  </si>
-  <si>
     <t>Complete</t>
   </si>
   <si>
@@ -182,10 +179,22 @@
     <t>Barbara</t>
   </si>
   <si>
-    <t>Lucas</t>
-  </si>
-  <si>
     <t>Dick</t>
+  </si>
+  <si>
+    <t>Butch</t>
+  </si>
+  <si>
+    <t>Harvey</t>
+  </si>
+  <si>
+    <t>Lucius</t>
+  </si>
+  <si>
+    <t>Lee</t>
+  </si>
+  <si>
+    <t>Carmine</t>
   </si>
 </sst>
 </file>
@@ -513,7 +522,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -543,21 +552,21 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L1" t="s">
         <v>0</v>
       </c>
       <c r="M1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -581,10 +590,10 @@
         <v>100000</v>
       </c>
       <c r="J2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L2">
         <v>10000</v>
@@ -595,10 +604,10 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
         <v>15</v>
@@ -622,10 +631,10 @@
         <v>10000000</v>
       </c>
       <c r="J3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L3">
         <v>2000</v>
@@ -636,10 +645,10 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
@@ -663,10 +672,10 @@
         <v>10000</v>
       </c>
       <c r="J4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L4">
         <v>50000</v>
@@ -677,10 +686,10 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
@@ -704,10 +713,10 @@
         <v>800000</v>
       </c>
       <c r="J5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L5">
         <v>3000</v>
@@ -736,13 +745,13 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -807,7 +816,7 @@
         <v>100000</v>
       </c>
       <c r="L2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -845,7 +854,7 @@
         <v>10000000</v>
       </c>
       <c r="L3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -883,12 +892,12 @@
         <v>10000</v>
       </c>
       <c r="L4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5">
         <v>1000</v>
@@ -897,7 +906,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5">
         <v>2000</v>
@@ -921,7 +930,7 @@
         <v>800000</v>
       </c>
       <c r="L5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -933,21 +942,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -979,7 +988,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2">
         <v>100000000</v>
@@ -988,7 +997,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E2">
         <v>1000</v>
@@ -1012,12 +1021,12 @@
         <v>100000</v>
       </c>
       <c r="L2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3">
         <v>100000000</v>
@@ -1026,7 +1035,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3">
         <v>4000</v>
@@ -1050,12 +1059,12 @@
         <v>10000000</v>
       </c>
       <c r="L3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B4">
         <v>100000000</v>
@@ -1064,7 +1073,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4">
         <v>1000</v>
@@ -1088,12 +1097,12 @@
         <v>10000</v>
       </c>
       <c r="L4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B5">
         <v>100000000</v>
@@ -1102,7 +1111,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5">
         <v>2000</v>
@@ -1126,7 +1135,7 @@
         <v>800000</v>
       </c>
       <c r="L5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1136,157 +1145,202 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2">
+        <v>100000000</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2">
+        <v>100</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>700</v>
+      </c>
+      <c r="J2">
+        <v>1920</v>
+      </c>
+      <c r="K2">
+        <v>99999</v>
+      </c>
+      <c r="L2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3">
+        <v>100000000</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
         <v>35</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3">
+        <v>100000</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>5000</v>
+      </c>
+      <c r="J3">
+        <v>1920</v>
+      </c>
+      <c r="K3">
+        <v>9999</v>
+      </c>
+      <c r="L3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4">
+        <v>100000000</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="C2">
-        <v>100</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>700</v>
-      </c>
-      <c r="G2">
-        <v>1920</v>
-      </c>
-      <c r="H2">
-        <v>99999</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="F4">
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>250</v>
+      </c>
+      <c r="J4">
+        <v>1960</v>
+      </c>
+      <c r="K4">
+        <v>9999</v>
+      </c>
+      <c r="L4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5">
+        <v>100000000</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" t="s">
         <v>15</v>
-      </c>
-      <c r="C3">
-        <v>100000</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>5000</v>
-      </c>
-      <c r="G3">
-        <v>1920</v>
-      </c>
-      <c r="H3">
-        <v>9999</v>
-      </c>
-      <c r="I3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>250</v>
-      </c>
-      <c r="G4">
-        <v>1960</v>
-      </c>
-      <c r="H4">
-        <v>9999</v>
-      </c>
-      <c r="I4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5">
-        <v>2000</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
       </c>
       <c r="F5">
         <v>2000</v>
       </c>
       <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>2000</v>
+      </c>
+      <c r="J5">
         <v>2010</v>
       </c>
-      <c r="H5">
+      <c r="K5">
         <v>800000</v>
       </c>
-      <c r="I5" t="s">
-        <v>19</v>
+      <c r="L5" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moved importEntities etc. to io.py; added self.listed (bool) to structures.Building();
Also required that entity specified for all technical.py processes.
</commit_message>
<xml_diff>
--- a/inputs/desaster_input_data_template.xlsx
+++ b/inputs/desaster_input_data_template.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geomando/Dropbox/github/SeaGrantSimulation/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geomando/Dropbox/github/DESaster/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="renters" sheetId="5" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="61">
   <si>
     <t>Savings</t>
   </si>
@@ -195,6 +195,24 @@
   </si>
   <si>
     <t>Carmine</t>
+  </si>
+  <si>
+    <t>For Sale</t>
+  </si>
+  <si>
+    <t>Listed</t>
+  </si>
+  <si>
+    <t>Greg</t>
+  </si>
+  <si>
+    <t>Allison</t>
+  </si>
+  <si>
+    <t>Rachel</t>
+  </si>
+  <si>
+    <t>Larry</t>
   </si>
 </sst>
 </file>
@@ -509,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -520,7 +538,7 @@
     <col min="10" max="10" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -560,8 +578,11 @@
       <c r="M1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -601,8 +622,11 @@
       <c r="M2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -642,8 +666,11 @@
       <c r="M3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -683,8 +710,11 @@
       <c r="M4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -722,6 +752,185 @@
         <v>3000</v>
       </c>
       <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <v>100</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>700</v>
+      </c>
+      <c r="H6">
+        <v>1920</v>
+      </c>
+      <c r="I6">
+        <v>99999</v>
+      </c>
+      <c r="J6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" t="s">
+        <v>57</v>
+      </c>
+      <c r="L6">
+        <v>100000000</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>100000</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>5000</v>
+      </c>
+      <c r="H7">
+        <v>1920</v>
+      </c>
+      <c r="I7">
+        <v>9999</v>
+      </c>
+      <c r="J7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K7" t="s">
+        <v>58</v>
+      </c>
+      <c r="L7">
+        <v>100000000</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>250</v>
+      </c>
+      <c r="H8">
+        <v>1960</v>
+      </c>
+      <c r="I8">
+        <v>9999</v>
+      </c>
+      <c r="J8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" t="s">
+        <v>59</v>
+      </c>
+      <c r="L8">
+        <v>100000000</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <v>2000</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>2000</v>
+      </c>
+      <c r="H9">
+        <v>2010</v>
+      </c>
+      <c r="I9">
+        <v>800000</v>
+      </c>
+      <c r="J9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" t="s">
+        <v>60</v>
+      </c>
+      <c r="L9">
+        <v>100000000</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9" t="b">
         <v>1</v>
       </c>
     </row>
@@ -732,10 +941,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:L5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -743,7 +952,7 @@
     <col min="12" max="12" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -780,8 +989,11 @@
       <c r="L1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -818,8 +1030,11 @@
       <c r="L2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -856,8 +1071,11 @@
       <c r="L3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -894,8 +1112,11 @@
       <c r="L4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -931,6 +1152,173 @@
       </c>
       <c r="L5" t="s">
         <v>18</v>
+      </c>
+      <c r="M5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6">
+        <v>100000000</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6">
+        <v>1000</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1100</v>
+      </c>
+      <c r="J6">
+        <v>1920</v>
+      </c>
+      <c r="K6">
+        <v>100000</v>
+      </c>
+      <c r="L6" t="s">
+        <v>44</v>
+      </c>
+      <c r="M6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7">
+        <v>100000000</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7">
+        <v>4000</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7">
+        <v>5000</v>
+      </c>
+      <c r="J7">
+        <v>1920</v>
+      </c>
+      <c r="K7">
+        <v>10000000</v>
+      </c>
+      <c r="L7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8">
+        <v>100000000</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8">
+        <v>1000</v>
+      </c>
+      <c r="F8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1200</v>
+      </c>
+      <c r="J8">
+        <v>1960</v>
+      </c>
+      <c r="K8">
+        <v>10000</v>
+      </c>
+      <c r="L8" t="s">
+        <v>45</v>
+      </c>
+      <c r="M8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9">
+        <v>100000000</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9">
+        <v>2000</v>
+      </c>
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>2000</v>
+      </c>
+      <c r="J9">
+        <v>2010</v>
+      </c>
+      <c r="K9">
+        <v>700000</v>
+      </c>
+      <c r="L9" t="s">
+        <v>18</v>
+      </c>
+      <c r="M9" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -943,7 +1331,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="L1" sqref="A1:L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1145,15 +1533,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -1190,8 +1578,11 @@
       <c r="L1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -1229,7 +1620,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -1267,7 +1658,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -1305,7 +1696,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
Completely separated io from model code (i.e., any assumptions about df or excel columns and format is now only in io.py)
</commit_message>
<xml_diff>
--- a/inputs/desaster_input_data_template.xlsx
+++ b/inputs/desaster_input_data_template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="63">
   <si>
     <t>Savings</t>
   </si>
@@ -197,9 +197,6 @@
     <t>Carmine</t>
   </si>
   <si>
-    <t>For Sale</t>
-  </si>
-  <si>
     <t>Listed</t>
   </si>
   <si>
@@ -213,16 +210,48 @@
   </si>
   <si>
     <t>Larry</t>
+  </si>
+  <si>
+    <t>Owner Savings</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>Latitude</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -245,13 +274,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -527,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="O1" sqref="O1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -538,7 +572,7 @@
     <col min="10" max="10" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -573,16 +607,22 @@
         <v>42</v>
       </c>
       <c r="L1" t="s">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="M1" t="s">
         <v>43</v>
       </c>
       <c r="N1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+      <c r="O1" t="s">
+        <v>61</v>
+      </c>
+      <c r="P1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -625,8 +665,14 @@
       <c r="N2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -669,8 +715,14 @@
       <c r="N3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -713,8 +765,14 @@
       <c r="N4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -757,8 +815,14 @@
       <c r="N5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -790,7 +854,7 @@
         <v>18</v>
       </c>
       <c r="K6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L6">
         <v>100000000</v>
@@ -801,8 +865,14 @@
       <c r="N6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -834,7 +904,7 @@
         <v>18</v>
       </c>
       <c r="K7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L7">
         <v>100000000</v>
@@ -845,8 +915,14 @@
       <c r="N7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -878,7 +954,7 @@
         <v>18</v>
       </c>
       <c r="K8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L8">
         <v>100000000</v>
@@ -889,8 +965,14 @@
       <c r="N8" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -922,7 +1004,7 @@
         <v>18</v>
       </c>
       <c r="K9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L9">
         <v>100000000</v>
@@ -932,6 +1014,12 @@
       </c>
       <c r="N9" t="b">
         <v>1</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -941,10 +1029,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -952,12 +1040,12 @@
     <col min="12" max="12" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="C1" t="s">
         <v>43</v>
@@ -990,10 +1078,16 @@
         <v>9</v>
       </c>
       <c r="M1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+      <c r="N1" t="s">
+        <v>61</v>
+      </c>
+      <c r="O1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1009,7 +1103,7 @@
       <c r="E2">
         <v>1000</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G2">
@@ -1033,8 +1127,14 @@
       <c r="M2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1074,8 +1174,14 @@
       <c r="M3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1115,8 +1221,14 @@
       <c r="M4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1156,8 +1268,14 @@
       <c r="M5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -1197,8 +1315,14 @@
       <c r="M6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>48</v>
       </c>
@@ -1238,8 +1362,14 @@
       <c r="M7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -1279,8 +1409,14 @@
       <c r="M8" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -1319,6 +1455,12 @@
       </c>
       <c r="M9" t="b">
         <v>1</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1328,15 +1470,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="A1:L5"/>
+      <selection activeCell="M1" sqref="M1:N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -1373,8 +1515,14 @@
       <c r="L1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1411,8 +1559,14 @@
       <c r="L2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1449,8 +1603,14 @@
       <c r="L3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -1487,8 +1647,14 @@
       <c r="L4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -1524,6 +1690,12 @@
       </c>
       <c r="L5" t="s">
         <v>18</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1533,15 +1705,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:L5"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -1579,10 +1751,13 @@
         <v>9</v>
       </c>
       <c r="M1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+      <c r="N1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -1619,8 +1794,14 @@
       <c r="L2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -1657,8 +1838,14 @@
       <c r="L3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -1695,8 +1882,14 @@
       <c r="L4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -1732,6 +1925,12 @@
       </c>
       <c r="L5" t="s">
         <v>18</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed financial.Loan to financial.LoanSBA; Created distributions.DurationDistributionHomeLoanSBA as a subclass of distributions.ProbabilityDistributions
</commit_message>
<xml_diff>
--- a/inputs/desaster_input_data_template.xlsx
+++ b/inputs/desaster_input_data_template.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="64">
   <si>
     <t>Savings</t>
   </si>
@@ -219,6 +219,9 @@
   </si>
   <si>
     <t>Latitude</t>
+  </si>
+  <si>
+    <t>Owner Credit</t>
   </si>
 </sst>
 </file>
@@ -561,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:P1048576"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -572,7 +575,7 @@
     <col min="10" max="10" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -621,8 +624,11 @@
       <c r="P1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -671,8 +677,11 @@
       <c r="P2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q2">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -721,8 +730,11 @@
       <c r="P3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q3">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -771,8 +783,11 @@
       <c r="P4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q4">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -821,8 +836,11 @@
       <c r="P5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q5">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -871,8 +889,11 @@
       <c r="P6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q6">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -921,8 +942,11 @@
       <c r="P7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q7">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -971,8 +995,11 @@
       <c r="P8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q8">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -1020,6 +1047,9 @@
       </c>
       <c r="P9">
         <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>700</v>
       </c>
     </row>
   </sheetData>
@@ -1029,10 +1059,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1040,7 +1070,7 @@
     <col min="12" max="12" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -1086,8 +1116,11 @@
       <c r="O1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1095,7 +1128,7 @@
         <v>5000</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -1122,7 +1155,7 @@
         <v>100000</v>
       </c>
       <c r="L2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="M2" t="b">
         <v>0</v>
@@ -1133,8 +1166,11 @@
       <c r="O2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1142,7 +1178,7 @@
         <v>250000</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="s">
         <v>14</v>
@@ -1180,8 +1216,11 @@
       <c r="O3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P3">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1189,7 +1228,7 @@
         <v>2500</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
@@ -1227,8 +1266,11 @@
       <c r="O4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P4">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1236,7 +1278,7 @@
         <v>1000</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="s">
         <v>20</v>
@@ -1263,7 +1305,7 @@
         <v>800000</v>
       </c>
       <c r="L5" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="M5" t="b">
         <v>0</v>
@@ -1274,8 +1316,11 @@
       <c r="O5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P5">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -1283,7 +1328,7 @@
         <v>100000000</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" t="s">
         <v>21</v>
@@ -1321,8 +1366,11 @@
       <c r="O6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P6">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>48</v>
       </c>
@@ -1330,7 +1378,7 @@
         <v>100000000</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" t="s">
         <v>22</v>
@@ -1368,8 +1416,11 @@
       <c r="O7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P7">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -1377,7 +1428,7 @@
         <v>100000000</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" t="s">
         <v>23</v>
@@ -1415,8 +1466,11 @@
       <c r="O8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P8">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -1424,7 +1478,7 @@
         <v>100000000</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" t="s">
         <v>24</v>
@@ -1461,6 +1515,9 @@
       </c>
       <c r="O9">
         <v>0</v>
+      </c>
+      <c r="P9">
+        <v>700</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Long duration if SBA > $25k; SBA filing deadline; insurance-loan-seq; insurance-loan-para
</commit_message>
<xml_diff>
--- a/inputs/desaster_input_data_template.xlsx
+++ b/inputs/desaster_input_data_template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="renters" sheetId="5" r:id="rId1"/>
@@ -566,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -666,7 +666,7 @@
         <v>10000</v>
       </c>
       <c r="M2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N2" t="b">
         <v>0</v>
@@ -719,7 +719,7 @@
         <v>2000</v>
       </c>
       <c r="M3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N3" t="b">
         <v>0</v>
@@ -1061,7 +1061,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Finished parallel in financial recovery policies; implemented write functions, etc.
</commit_message>
<xml_diff>
--- a/inputs/desaster_input_data_template.xlsx
+++ b/inputs/desaster_input_data_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="renters" sheetId="5" r:id="rId1"/>
@@ -566,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -663,7 +663,7 @@
         <v>38</v>
       </c>
       <c r="L2">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -716,7 +716,7 @@
         <v>39</v>
       </c>
       <c r="L3">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -769,7 +769,7 @@
         <v>40</v>
       </c>
       <c r="L4">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="M4">
         <v>1</v>
@@ -822,7 +822,7 @@
         <v>41</v>
       </c>
       <c r="L5">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="M5">
         <v>1</v>
@@ -1061,8 +1061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1125,7 +1125,7 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1155,7 +1155,7 @@
         <v>100000</v>
       </c>
       <c r="L2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="M2" t="b">
         <v>0</v>
@@ -1167,7 +1167,7 @@
         <v>0</v>
       </c>
       <c r="P2">
-        <v>500</v>
+        <v>700</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
@@ -1175,7 +1175,7 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>250000</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1205,7 +1205,7 @@
         <v>10000000</v>
       </c>
       <c r="L3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="M3" t="b">
         <v>0</v>
@@ -1225,7 +1225,7 @@
         <v>16</v>
       </c>
       <c r="B4">
-        <v>2500</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1255,7 +1255,7 @@
         <v>10000</v>
       </c>
       <c r="L4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M4" t="b">
         <v>0</v>
@@ -1275,7 +1275,7 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1305,7 +1305,7 @@
         <v>800000</v>
       </c>
       <c r="L5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M5" t="b">
         <v>0</v>
@@ -1405,7 +1405,7 @@
         <v>10000000</v>
       </c>
       <c r="L7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="M7" t="b">
         <v>1</v>
@@ -1455,7 +1455,7 @@
         <v>10000</v>
       </c>
       <c r="L8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M8" t="b">
         <v>1</v>
@@ -1505,7 +1505,7 @@
         <v>700000</v>
       </c>
       <c r="L9" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="M9" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Made recovery_funds a container, implemented prior_residences/properties[0] in entity.replace_home()
</commit_message>
<xml_diff>
--- a/inputs/desaster_input_data_template.xlsx
+++ b/inputs/desaster_input_data_template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -1062,7 +1062,7 @@
   <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L9"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1125,7 +1125,7 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1175,7 +1175,7 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1225,7 +1225,7 @@
         <v>16</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1275,7 +1275,7 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C5">
         <v>0</v>

</xml_diff>

<commit_message>
added np.pv, area_pct, room_tol, closing_time, notice_time, income, move-in cost
</commit_message>
<xml_diff>
--- a/inputs/desaster_input_data_template.xlsx
+++ b/inputs/desaster_input_data_template.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="70">
   <si>
     <t>Savings</t>
   </si>
@@ -222,6 +222,24 @@
   </si>
   <si>
     <t>Owner Credit</t>
+  </si>
+  <si>
+    <t>Tenant Savings</t>
+  </si>
+  <si>
+    <t>Tenant Credit</t>
+  </si>
+  <si>
+    <t>Tenant Insurance</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Monthly Cost</t>
+  </si>
+  <si>
+    <t>Income</t>
   </si>
 </sst>
 </file>
@@ -282,9 +300,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="38" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -564,18 +583,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="10" max="10" width="16.83203125" customWidth="1"/>
+    <col min="14" max="14" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -586,49 +605,61 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>69</v>
       </c>
       <c r="E1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="O1" t="s">
         <v>42</v>
       </c>
-      <c r="L1" t="s">
+      <c r="P1" t="s">
         <v>60</v>
       </c>
-      <c r="M1" t="s">
+      <c r="Q1" t="s">
         <v>43</v>
       </c>
-      <c r="N1" t="s">
+      <c r="R1" t="s">
         <v>55</v>
       </c>
-      <c r="O1" t="s">
+      <c r="S1" t="s">
         <v>61</v>
       </c>
-      <c r="P1" t="s">
+      <c r="T1" t="s">
         <v>62</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="U1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -639,49 +670,63 @@
         <v>12</v>
       </c>
       <c r="D2">
+        <v>50000</v>
+      </c>
+      <c r="E2">
         <v>1000</v>
       </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
       <c r="F2">
-        <v>1</v>
+        <v>700</v>
       </c>
       <c r="G2">
-        <v>700</v>
+        <v>0</v>
       </c>
       <c r="H2">
+        <f>2.48*K2</f>
+        <v>2480</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1000</v>
+      </c>
+      <c r="L2">
         <v>1920</v>
       </c>
-      <c r="I2">
-        <v>100000</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="M2">
+        <f>279*K2</f>
+        <v>279000</v>
+      </c>
+      <c r="N2" t="s">
         <v>18</v>
       </c>
-      <c r="K2" t="s">
+      <c r="O2" t="s">
         <v>38</v>
       </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2" t="b">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
       <c r="P2">
         <v>0</v>
       </c>
       <c r="Q2">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="R2" t="b">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -692,49 +737,63 @@
         <v>15</v>
       </c>
       <c r="D3">
-        <v>3000</v>
+        <v>1000000</v>
       </c>
       <c r="E3">
+        <v>1000</v>
+      </c>
+      <c r="F3">
+        <v>700</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H9" si="0">2.48*K3</f>
+        <v>3720</v>
+      </c>
+      <c r="I3">
         <v>3</v>
       </c>
-      <c r="F3">
+      <c r="J3">
         <v>2</v>
       </c>
-      <c r="G3">
-        <v>5000</v>
-      </c>
-      <c r="H3">
+      <c r="K3">
+        <v>1500</v>
+      </c>
+      <c r="L3">
         <v>1920</v>
       </c>
-      <c r="I3">
-        <v>10000000</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="M3">
+        <f t="shared" ref="M3:M9" si="1">279*K3</f>
+        <v>418500</v>
+      </c>
+      <c r="N3" t="s">
         <v>18</v>
       </c>
-      <c r="K3" t="s">
+      <c r="O3" t="s">
         <v>39</v>
       </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3" t="b">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
       <c r="P3">
         <v>0</v>
       </c>
       <c r="Q3">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="R3" t="b">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -745,49 +804,63 @@
         <v>15</v>
       </c>
       <c r="D4">
-        <v>750</v>
+        <v>25000</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>700</v>
       </c>
       <c r="G4">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="H4">
+        <f t="shared" si="0"/>
+        <v>1240</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>500</v>
+      </c>
+      <c r="L4">
         <v>1960</v>
       </c>
-      <c r="I4">
-        <v>10000</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="M4">
+        <f t="shared" si="1"/>
+        <v>139500</v>
+      </c>
+      <c r="N4" t="s">
         <v>18</v>
       </c>
-      <c r="K4" t="s">
+      <c r="O4" t="s">
         <v>40</v>
       </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-      <c r="N4" t="b">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
       <c r="P4">
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="R4" t="b">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -798,49 +871,63 @@
         <v>15</v>
       </c>
       <c r="D5">
-        <v>1500</v>
+        <v>100000</v>
       </c>
       <c r="E5">
+        <v>1000</v>
+      </c>
+      <c r="F5">
+        <v>700</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>4960</v>
+      </c>
+      <c r="I5">
         <v>2</v>
       </c>
-      <c r="F5">
+      <c r="J5">
         <v>2</v>
       </c>
-      <c r="G5">
+      <c r="K5">
         <v>2000</v>
       </c>
-      <c r="H5">
+      <c r="L5">
         <v>2010</v>
       </c>
-      <c r="I5">
-        <v>800000</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="M5">
+        <f t="shared" si="1"/>
+        <v>558000</v>
+      </c>
+      <c r="N5" t="s">
         <v>18</v>
       </c>
-      <c r="K5" t="s">
+      <c r="O5" t="s">
         <v>41</v>
       </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="N5" t="b">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
       <c r="P5">
         <v>0</v>
       </c>
       <c r="Q5">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="R5" t="b">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -851,49 +938,63 @@
         <v>12</v>
       </c>
       <c r="D6">
-        <v>100</v>
+        <v>100000000</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>700</v>
       </c>
       <c r="G6">
-        <v>700</v>
+        <v>0</v>
       </c>
       <c r="H6">
+        <f t="shared" si="0"/>
+        <v>2480</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1000</v>
+      </c>
+      <c r="L6">
         <v>1920</v>
       </c>
-      <c r="I6">
-        <v>99999</v>
-      </c>
-      <c r="J6" t="s">
-        <v>18</v>
-      </c>
-      <c r="K6" t="s">
+      <c r="M6">
+        <f t="shared" si="1"/>
+        <v>279000</v>
+      </c>
+      <c r="N6" t="s">
+        <v>67</v>
+      </c>
+      <c r="O6" t="s">
         <v>56</v>
       </c>
-      <c r="L6">
-        <v>100000000</v>
-      </c>
-      <c r="M6">
-        <v>1</v>
-      </c>
-      <c r="N6" t="b">
-        <v>1</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
       <c r="P6">
-        <v>0</v>
+        <v>100000000</v>
       </c>
       <c r="Q6">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="R6" t="b">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -904,49 +1005,63 @@
         <v>15</v>
       </c>
       <c r="D7">
-        <v>100000</v>
+        <v>100000000</v>
       </c>
       <c r="E7">
+        <v>1000</v>
+      </c>
+      <c r="F7">
+        <v>700</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>3720</v>
+      </c>
+      <c r="I7">
         <v>2</v>
       </c>
-      <c r="F7">
+      <c r="J7">
         <v>2</v>
       </c>
-      <c r="G7">
-        <v>5000</v>
-      </c>
-      <c r="H7">
+      <c r="K7">
+        <v>1500</v>
+      </c>
+      <c r="L7">
         <v>1920</v>
       </c>
-      <c r="I7">
-        <v>9999</v>
-      </c>
-      <c r="J7" t="s">
-        <v>18</v>
-      </c>
-      <c r="K7" t="s">
+      <c r="M7">
+        <f t="shared" si="1"/>
+        <v>418500</v>
+      </c>
+      <c r="N7" t="s">
+        <v>67</v>
+      </c>
+      <c r="O7" t="s">
         <v>57</v>
       </c>
-      <c r="L7">
-        <v>100000000</v>
-      </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
-      <c r="N7" t="b">
-        <v>1</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
       <c r="P7">
-        <v>0</v>
+        <v>100000000</v>
       </c>
       <c r="Q7">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="R7" t="b">
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -957,49 +1072,63 @@
         <v>12</v>
       </c>
       <c r="D8">
-        <v>10</v>
+        <v>100000000</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>700</v>
       </c>
       <c r="G8">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="H8">
+        <f t="shared" si="0"/>
+        <v>1240</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>500</v>
+      </c>
+      <c r="L8">
         <v>1960</v>
       </c>
-      <c r="I8">
-        <v>9999</v>
-      </c>
-      <c r="J8" t="s">
-        <v>18</v>
-      </c>
-      <c r="K8" t="s">
+      <c r="M8">
+        <f t="shared" si="1"/>
+        <v>139500</v>
+      </c>
+      <c r="N8" t="s">
+        <v>67</v>
+      </c>
+      <c r="O8" t="s">
         <v>58</v>
       </c>
-      <c r="L8">
-        <v>100000000</v>
-      </c>
-      <c r="M8">
-        <v>1</v>
-      </c>
-      <c r="N8" t="b">
-        <v>1</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
       <c r="P8">
-        <v>0</v>
+        <v>100000000</v>
       </c>
       <c r="Q8">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="R8" t="b">
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -1010,45 +1139,59 @@
         <v>15</v>
       </c>
       <c r="D9">
+        <v>100000000</v>
+      </c>
+      <c r="E9">
+        <v>1000</v>
+      </c>
+      <c r="F9">
+        <v>700</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>4960</v>
+      </c>
+      <c r="I9">
+        <v>3</v>
+      </c>
+      <c r="J9">
+        <v>2</v>
+      </c>
+      <c r="K9">
         <v>2000</v>
       </c>
-      <c r="E9">
-        <v>3</v>
-      </c>
-      <c r="F9">
-        <v>2</v>
-      </c>
-      <c r="G9">
-        <v>2000</v>
-      </c>
-      <c r="H9">
+      <c r="L9">
         <v>2010</v>
       </c>
-      <c r="I9">
-        <v>800000</v>
-      </c>
-      <c r="J9" t="s">
-        <v>18</v>
-      </c>
-      <c r="K9" t="s">
+      <c r="M9">
+        <f t="shared" si="1"/>
+        <v>558000</v>
+      </c>
+      <c r="N9" t="s">
+        <v>67</v>
+      </c>
+      <c r="O9" t="s">
         <v>59</v>
       </c>
-      <c r="L9">
-        <v>100000000</v>
-      </c>
-      <c r="M9">
-        <v>1</v>
-      </c>
-      <c r="N9" t="b">
-        <v>1</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
       <c r="P9">
-        <v>0</v>
+        <v>100000000</v>
       </c>
       <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="R9" t="b">
+        <v>1</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
         <v>700</v>
       </c>
     </row>
@@ -1059,268 +1202,291 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="12" max="12" width="16.83203125" customWidth="1"/>
+    <col min="13" max="13" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>33</v>
       </c>
       <c r="B1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" t="s">
         <v>60</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>43</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>55</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>61</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>62</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2">
+        <v>60000</v>
+      </c>
+      <c r="C2">
         <v>100</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="E2">
-        <v>1000</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2">
+        <f>-PMT(0.05/12,360,(L2-L2*0.1),0)</f>
+        <v>1482.7550049218294</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
       <c r="H2">
         <v>1</v>
       </c>
       <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
         <v>1100</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>1920</v>
       </c>
-      <c r="K2">
-        <v>100000</v>
-      </c>
-      <c r="L2" t="s">
-        <v>44</v>
-      </c>
-      <c r="M2" t="b">
-        <v>0</v>
-      </c>
-      <c r="N2">
+      <c r="L2">
+        <f>J2*279</f>
+        <v>306900</v>
+      </c>
+      <c r="M2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" t="b">
         <v>0</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
       <c r="B3">
+        <v>1000000</v>
+      </c>
+      <c r="C3">
         <v>100</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="E3">
-        <v>4000</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2">
+        <f t="shared" ref="F3:F9" si="0">-PMT(0.05/12,360,(L3-L3*0.1),0)</f>
+        <v>4043.8772861504435</v>
+      </c>
+      <c r="G3" t="s">
         <v>15</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>4</v>
       </c>
-      <c r="H3">
-        <v>5</v>
-      </c>
       <c r="I3">
-        <v>5000</v>
+        <v>3</v>
       </c>
       <c r="J3">
+        <v>3000</v>
+      </c>
+      <c r="K3">
         <v>1920</v>
       </c>
-      <c r="K3">
-        <v>10000000</v>
-      </c>
-      <c r="L3" t="s">
-        <v>44</v>
-      </c>
-      <c r="M3" t="b">
-        <v>0</v>
-      </c>
-      <c r="N3">
+      <c r="L3">
+        <f t="shared" ref="L3:L5" si="1">J3*279</f>
+        <v>837000</v>
+      </c>
+      <c r="M3" t="s">
+        <v>45</v>
+      </c>
+      <c r="N3" t="b">
         <v>0</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
       <c r="B4">
+        <v>45000</v>
+      </c>
+      <c r="C4">
         <v>100</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="E4">
-        <v>1000</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="F4" s="2">
+        <f t="shared" si="0"/>
+        <v>1010.9693215376109</v>
+      </c>
+      <c r="G4" t="s">
         <v>15</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>2</v>
       </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
       <c r="I4">
-        <v>1200</v>
+        <v>1</v>
       </c>
       <c r="J4">
+        <v>750</v>
+      </c>
+      <c r="K4">
         <v>1960</v>
       </c>
-      <c r="K4">
-        <v>10000</v>
-      </c>
-      <c r="L4" t="s">
-        <v>44</v>
-      </c>
-      <c r="M4" t="b">
-        <v>0</v>
-      </c>
-      <c r="N4">
+      <c r="L4">
+        <f t="shared" si="1"/>
+        <v>209250</v>
+      </c>
+      <c r="M4" t="s">
+        <v>46</v>
+      </c>
+      <c r="N4" t="b">
         <v>0</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
       <c r="B5">
+        <v>125000</v>
+      </c>
+      <c r="C5">
         <v>100</v>
       </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
         <v>20</v>
       </c>
-      <c r="E5">
+      <c r="F5" s="2">
+        <f t="shared" si="0"/>
+        <v>2695.9181907669627</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
         <v>2000</v>
       </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5">
-        <v>3</v>
-      </c>
-      <c r="H5">
-        <v>2</v>
-      </c>
-      <c r="I5">
-        <v>2000</v>
-      </c>
-      <c r="J5">
+      <c r="K5">
         <v>2010</v>
       </c>
-      <c r="K5">
-        <v>800000</v>
-      </c>
-      <c r="L5" t="s">
+      <c r="L5">
+        <f t="shared" si="1"/>
+        <v>558000</v>
+      </c>
+      <c r="M5" t="s">
         <v>44</v>
       </c>
-      <c r="M5" t="b">
-        <v>0</v>
-      </c>
-      <c r="N5">
+      <c r="N5" t="b">
         <v>0</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -1328,49 +1494,53 @@
         <v>100000000</v>
       </c>
       <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6" t="s">
+        <v>100000000</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
         <v>21</v>
       </c>
-      <c r="E6">
-        <v>1000</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="F6" s="2">
+        <f t="shared" si="0"/>
+        <v>1449.4183821327754</v>
+      </c>
+      <c r="G6" t="s">
         <v>12</v>
       </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
       <c r="H6">
         <v>1</v>
       </c>
       <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
         <v>1100</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>1920</v>
       </c>
-      <c r="K6">
-        <v>100000</v>
-      </c>
-      <c r="L6" t="s">
-        <v>44</v>
-      </c>
-      <c r="M6" t="b">
-        <v>1</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
+      <c r="L6">
+        <v>300000</v>
+      </c>
+      <c r="M6" t="s">
+        <v>67</v>
+      </c>
+      <c r="N6" t="b">
+        <v>1</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>48</v>
       </c>
@@ -1378,49 +1548,53 @@
         <v>100000000</v>
       </c>
       <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7" t="s">
+        <v>100000000</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
         <v>22</v>
       </c>
-      <c r="E7">
-        <v>4000</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="F7" s="2">
+        <f t="shared" si="0"/>
+        <v>3865.1156856874013</v>
+      </c>
+      <c r="G7" t="s">
         <v>15</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>4</v>
       </c>
-      <c r="H7">
-        <v>5</v>
-      </c>
       <c r="I7">
-        <v>5000</v>
+        <v>3</v>
       </c>
       <c r="J7">
+        <v>3000</v>
+      </c>
+      <c r="K7">
         <v>1920</v>
       </c>
-      <c r="K7">
-        <v>10000000</v>
-      </c>
-      <c r="L7" t="s">
-        <v>44</v>
-      </c>
-      <c r="M7" t="b">
-        <v>1</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
+      <c r="L7">
+        <v>800000</v>
+      </c>
+      <c r="M7" t="s">
+        <v>67</v>
+      </c>
+      <c r="N7" t="b">
+        <v>1</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -1428,49 +1602,53 @@
         <v>100000000</v>
       </c>
       <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8" t="s">
+        <v>100000000</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
         <v>23</v>
       </c>
-      <c r="E8">
-        <v>1000</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="F8" s="2">
+        <f t="shared" si="0"/>
+        <v>1449.4183821327754</v>
+      </c>
+      <c r="G8" t="s">
         <v>15</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>2</v>
       </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
       <c r="I8">
-        <v>1200</v>
+        <v>1</v>
       </c>
       <c r="J8">
+        <v>750</v>
+      </c>
+      <c r="K8">
         <v>1960</v>
       </c>
-      <c r="K8">
-        <v>10000</v>
-      </c>
-      <c r="L8" t="s">
-        <v>44</v>
-      </c>
-      <c r="M8" t="b">
-        <v>1</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
+      <c r="L8">
+        <v>300000</v>
+      </c>
+      <c r="M8" t="s">
+        <v>67</v>
+      </c>
+      <c r="N8" t="b">
+        <v>1</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -1478,45 +1656,49 @@
         <v>100000000</v>
       </c>
       <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9" t="s">
+        <v>100000000</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
         <v>24</v>
       </c>
-      <c r="E9">
+      <c r="F9" s="2">
+        <f t="shared" si="0"/>
+        <v>2415.6973035546257</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="J9">
         <v>2000</v>
       </c>
-      <c r="F9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9">
-        <v>3</v>
-      </c>
-      <c r="H9">
-        <v>2</v>
-      </c>
-      <c r="I9">
-        <v>2000</v>
-      </c>
-      <c r="J9">
+      <c r="K9">
         <v>2010</v>
       </c>
-      <c r="K9">
-        <v>700000</v>
-      </c>
-      <c r="L9" t="s">
-        <v>44</v>
-      </c>
-      <c r="M9" t="b">
-        <v>1</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
+      <c r="L9">
+        <v>500000</v>
+      </c>
+      <c r="M9" t="s">
+        <v>67</v>
+      </c>
+      <c r="N9" t="b">
+        <v>1</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
       <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
         <v>700</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Got renters working again; added folium to notebook
</commit_message>
<xml_diff>
--- a/inputs/desaster_input_data_template.xlsx
+++ b/inputs/desaster_input_data_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="renters" sheetId="5" r:id="rId1"/>
@@ -585,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -670,7 +670,8 @@
         <v>12</v>
       </c>
       <c r="D2">
-        <v>50000</v>
+        <f>12*H2/0.25</f>
+        <v>119040</v>
       </c>
       <c r="E2">
         <v>1000</v>
@@ -702,13 +703,13 @@
         <v>279000</v>
       </c>
       <c r="N2" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="O2" t="s">
         <v>38</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -717,10 +718,10 @@
         <v>0</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>-90.294238000000007</v>
       </c>
       <c r="T2">
-        <v>0</v>
+        <v>43.224015000000001</v>
       </c>
       <c r="U2">
         <v>700</v>
@@ -737,7 +738,8 @@
         <v>15</v>
       </c>
       <c r="D3">
-        <v>1000000</v>
+        <f t="shared" ref="D3:D5" si="0">12*H3/0.25</f>
+        <v>178560</v>
       </c>
       <c r="E3">
         <v>1000</v>
@@ -749,7 +751,7 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H9" si="0">2.48*K3</f>
+        <f t="shared" ref="H3:H9" si="1">2.48*K3</f>
         <v>3720</v>
       </c>
       <c r="I3">
@@ -765,17 +767,17 @@
         <v>1920</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M9" si="1">279*K3</f>
+        <f t="shared" ref="M3:M9" si="2">279*K3</f>
         <v>418500</v>
       </c>
       <c r="N3" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="O3" t="s">
         <v>39</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -784,10 +786,10 @@
         <v>0</v>
       </c>
       <c r="S3">
-        <v>0</v>
+        <v>-90.293766000000005</v>
       </c>
       <c r="T3">
-        <v>0</v>
+        <v>43.224062000000004</v>
       </c>
       <c r="U3">
         <v>700</v>
@@ -804,7 +806,8 @@
         <v>15</v>
       </c>
       <c r="D4">
-        <v>25000</v>
+        <f t="shared" si="0"/>
+        <v>59520</v>
       </c>
       <c r="E4">
         <v>1000</v>
@@ -816,7 +819,7 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1240</v>
       </c>
       <c r="I4">
@@ -832,17 +835,17 @@
         <v>1960</v>
       </c>
       <c r="M4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>139500</v>
       </c>
       <c r="N4" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="O4" t="s">
         <v>40</v>
       </c>
       <c r="P4">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="Q4">
         <v>1</v>
@@ -851,10 +854,10 @@
         <v>0</v>
       </c>
       <c r="S4">
-        <v>0</v>
+        <v>-90.293294000000003</v>
       </c>
       <c r="T4">
-        <v>0</v>
+        <v>43.224125000000001</v>
       </c>
       <c r="U4">
         <v>700</v>
@@ -871,7 +874,8 @@
         <v>15</v>
       </c>
       <c r="D5">
-        <v>100000</v>
+        <f t="shared" si="0"/>
+        <v>238080</v>
       </c>
       <c r="E5">
         <v>1000</v>
@@ -883,7 +887,7 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4960</v>
       </c>
       <c r="I5">
@@ -899,7 +903,7 @@
         <v>2010</v>
       </c>
       <c r="M5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>558000</v>
       </c>
       <c r="N5" t="s">
@@ -909,7 +913,7 @@
         <v>41</v>
       </c>
       <c r="P5">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="Q5">
         <v>1</v>
@@ -918,10 +922,10 @@
         <v>0</v>
       </c>
       <c r="S5">
-        <v>0</v>
+        <v>-90.293058000000002</v>
       </c>
       <c r="T5">
-        <v>0</v>
+        <v>43.223936999999999</v>
       </c>
       <c r="U5">
         <v>700</v>
@@ -950,7 +954,7 @@
         <v>0</v>
       </c>
       <c r="H6">
-        <f t="shared" si="0"/>
+        <f>2.48*K6</f>
         <v>2480</v>
       </c>
       <c r="I6">
@@ -966,7 +970,7 @@
         <v>1920</v>
       </c>
       <c r="M6">
-        <f t="shared" si="1"/>
+        <f>279*K6</f>
         <v>279000</v>
       </c>
       <c r="N6" t="s">
@@ -985,10 +989,10 @@
         <v>1</v>
       </c>
       <c r="S6">
-        <v>0</v>
+        <v>-90.293080000000003</v>
       </c>
       <c r="T6">
-        <v>0</v>
+        <v>43.223671000000003</v>
       </c>
       <c r="U6">
         <v>700</v>
@@ -1017,11 +1021,11 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="H7:H9" si="3">2.48*K7</f>
         <v>3720</v>
       </c>
       <c r="I7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J7">
         <v>2</v>
@@ -1033,7 +1037,7 @@
         <v>1920</v>
       </c>
       <c r="M7">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="M7:M9" si="4">279*K7</f>
         <v>418500</v>
       </c>
       <c r="N7" t="s">
@@ -1052,10 +1056,10 @@
         <v>1</v>
       </c>
       <c r="S7">
-        <v>0</v>
+        <v>-90.292736000000005</v>
       </c>
       <c r="T7">
-        <v>0</v>
+        <v>43.223545999999999</v>
       </c>
       <c r="U7">
         <v>700</v>
@@ -1069,7 +1073,7 @@
         <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D8">
         <v>100000000</v>
@@ -1084,7 +1088,7 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1240</v>
       </c>
       <c r="I8">
@@ -1100,7 +1104,7 @@
         <v>1960</v>
       </c>
       <c r="M8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>139500</v>
       </c>
       <c r="N8" t="s">
@@ -1119,10 +1123,10 @@
         <v>1</v>
       </c>
       <c r="S8">
-        <v>0</v>
+        <v>-90.296190999999993</v>
       </c>
       <c r="T8">
-        <v>0</v>
+        <v>43.223405999999997</v>
       </c>
       <c r="U8">
         <v>700</v>
@@ -1151,11 +1155,11 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>4960</v>
       </c>
       <c r="I9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J9">
         <v>2</v>
@@ -1167,7 +1171,7 @@
         <v>2010</v>
       </c>
       <c r="M9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>558000</v>
       </c>
       <c r="N9" t="s">
@@ -1186,10 +1190,10 @@
         <v>1</v>
       </c>
       <c r="S9">
-        <v>0</v>
+        <v>-90.295739999999995</v>
       </c>
       <c r="T9">
-        <v>0</v>
+        <v>43.223359000000002</v>
       </c>
       <c r="U9">
         <v>700</v>
@@ -1204,8 +1208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1312,10 +1316,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>-90.296126999999998</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>43.224344000000002</v>
       </c>
       <c r="Q2">
         <v>700</v>
@@ -1367,10 +1371,10 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>0</v>
+        <v>-90.295697000000004</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <v>43.224218999999998</v>
       </c>
       <c r="Q3">
         <v>700</v>
@@ -1422,10 +1426,10 @@
         <v>0</v>
       </c>
       <c r="O4">
-        <v>0</v>
+        <v>-90.296706</v>
       </c>
       <c r="P4">
-        <v>0</v>
+        <v>43.223984000000002</v>
       </c>
       <c r="Q4">
         <v>700</v>
@@ -1477,10 +1481,10 @@
         <v>0</v>
       </c>
       <c r="O5">
-        <v>0</v>
+        <v>-90.296642000000006</v>
       </c>
       <c r="P5">
-        <v>0</v>
+        <v>43.223750000000003</v>
       </c>
       <c r="Q5">
         <v>700</v>
@@ -1531,10 +1535,10 @@
         <v>1</v>
       </c>
       <c r="O6">
-        <v>0</v>
+        <v>-90.295053999999993</v>
       </c>
       <c r="P6">
-        <v>0</v>
+        <v>43.224375000000002</v>
       </c>
       <c r="Q6">
         <v>700</v>
@@ -1585,10 +1589,10 @@
         <v>1</v>
       </c>
       <c r="O7">
-        <v>0</v>
+        <v>-90.294539</v>
       </c>
       <c r="P7">
-        <v>0</v>
+        <v>43.224390999999997</v>
       </c>
       <c r="Q7">
         <v>700</v>
@@ -1639,10 +1643,10 @@
         <v>1</v>
       </c>
       <c r="O8">
-        <v>0</v>
+        <v>-90.295225000000002</v>
       </c>
       <c r="P8">
-        <v>0</v>
+        <v>43.223953000000002</v>
       </c>
       <c r="Q8">
         <v>700</v>
@@ -1693,10 +1697,10 @@
         <v>1</v>
       </c>
       <c r="O9">
-        <v>0</v>
+        <v>-90.295225000000002</v>
       </c>
       <c r="P9">
-        <v>0</v>
+        <v>43.223717999999998</v>
       </c>
       <c r="Q9">
         <v>700</v>

</xml_diff>

<commit_message>
Fxns: dashboard, folium_map, Insurance_FirstThen_IA_SBA_Parallel
</commit_message>
<xml_diff>
--- a/inputs/desaster_input_data_template.xlsx
+++ b/inputs/desaster_input_data_template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="renters" sheetId="5" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="73">
   <si>
     <t>Savings</t>
   </si>
@@ -240,6 +240,15 @@
   </si>
   <si>
     <t>Income</t>
+  </si>
+  <si>
+    <t>Tenure</t>
+  </si>
+  <si>
+    <t>Rental</t>
+  </si>
+  <si>
+    <t>Owner Occupied</t>
   </si>
 </sst>
 </file>
@@ -583,10 +592,660 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U9"/>
+  <dimension ref="A1:V9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="15" max="15" width="16.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>60</v>
+      </c>
+      <c r="R1" t="s">
+        <v>43</v>
+      </c>
+      <c r="S1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T1" t="s">
+        <v>61</v>
+      </c>
+      <c r="U1" t="s">
+        <v>62</v>
+      </c>
+      <c r="V1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2">
+        <f>12*I2/0.25</f>
+        <v>119040</v>
+      </c>
+      <c r="F2">
+        <v>1000</v>
+      </c>
+      <c r="G2">
+        <v>700</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <f>2.48*L2</f>
+        <v>2480</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1000</v>
+      </c>
+      <c r="M2">
+        <v>1920</v>
+      </c>
+      <c r="N2">
+        <f>279*L2</f>
+        <v>279000</v>
+      </c>
+      <c r="O2" t="s">
+        <v>45</v>
+      </c>
+      <c r="P2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q2">
+        <v>30000</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2" t="b">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>-90.294238000000007</v>
+      </c>
+      <c r="U2">
+        <v>43.224015000000001</v>
+      </c>
+      <c r="V2">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E5" si="0">12*I3/0.25</f>
+        <v>178560</v>
+      </c>
+      <c r="F3">
+        <v>1000</v>
+      </c>
+      <c r="G3">
+        <v>700</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I5" si="1">2.48*L3</f>
+        <v>3720</v>
+      </c>
+      <c r="J3">
+        <v>3</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>1500</v>
+      </c>
+      <c r="M3">
+        <v>1920</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N5" si="2">279*L3</f>
+        <v>418500</v>
+      </c>
+      <c r="O3" t="s">
+        <v>44</v>
+      </c>
+      <c r="P3" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q3">
+        <v>30000</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3" t="b">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>-90.293766000000005</v>
+      </c>
+      <c r="U3">
+        <v>43.224062000000004</v>
+      </c>
+      <c r="V3">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>59520</v>
+      </c>
+      <c r="F4">
+        <v>1000</v>
+      </c>
+      <c r="G4">
+        <v>700</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>1240</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>500</v>
+      </c>
+      <c r="M4">
+        <v>1960</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="2"/>
+        <v>139500</v>
+      </c>
+      <c r="O4" t="s">
+        <v>46</v>
+      </c>
+      <c r="P4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q4">
+        <v>30000</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4" t="b">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>-90.293294000000003</v>
+      </c>
+      <c r="U4">
+        <v>43.224125000000001</v>
+      </c>
+      <c r="V4">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>238080</v>
+      </c>
+      <c r="F5">
+        <v>1000</v>
+      </c>
+      <c r="G5">
+        <v>700</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>4960</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>2000</v>
+      </c>
+      <c r="M5">
+        <v>2010</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="2"/>
+        <v>558000</v>
+      </c>
+      <c r="O5" t="s">
+        <v>18</v>
+      </c>
+      <c r="P5" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q5">
+        <v>30000</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5" t="b">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>-90.293058000000002</v>
+      </c>
+      <c r="U5">
+        <v>43.223936999999999</v>
+      </c>
+      <c r="V5">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6">
+        <v>100000000</v>
+      </c>
+      <c r="F6">
+        <v>1000</v>
+      </c>
+      <c r="G6">
+        <v>700</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <f>2.48*L6</f>
+        <v>2480</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1000</v>
+      </c>
+      <c r="M6">
+        <v>1920</v>
+      </c>
+      <c r="N6">
+        <f>279*L6</f>
+        <v>279000</v>
+      </c>
+      <c r="O6" t="s">
+        <v>67</v>
+      </c>
+      <c r="P6" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q6">
+        <v>100000000</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6" t="b">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>-90.293080000000003</v>
+      </c>
+      <c r="U6">
+        <v>43.223671000000003</v>
+      </c>
+      <c r="V6">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7">
+        <v>100000000</v>
+      </c>
+      <c r="F7">
+        <v>1000</v>
+      </c>
+      <c r="G7">
+        <v>700</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <f t="shared" ref="I7:I9" si="3">2.48*L7</f>
+        <v>3720</v>
+      </c>
+      <c r="J7">
+        <v>3</v>
+      </c>
+      <c r="K7">
+        <v>2</v>
+      </c>
+      <c r="L7">
+        <v>1500</v>
+      </c>
+      <c r="M7">
+        <v>1920</v>
+      </c>
+      <c r="N7">
+        <f t="shared" ref="N7:N9" si="4">279*L7</f>
+        <v>418500</v>
+      </c>
+      <c r="O7" t="s">
+        <v>67</v>
+      </c>
+      <c r="P7" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q7">
+        <v>100000000</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7" t="b">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>-90.292736000000005</v>
+      </c>
+      <c r="U7">
+        <v>43.223545999999999</v>
+      </c>
+      <c r="V7">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8">
+        <v>100000000</v>
+      </c>
+      <c r="F8">
+        <v>1000</v>
+      </c>
+      <c r="G8">
+        <v>700</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="3"/>
+        <v>1240</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>500</v>
+      </c>
+      <c r="M8">
+        <v>1960</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="4"/>
+        <v>139500</v>
+      </c>
+      <c r="O8" t="s">
+        <v>67</v>
+      </c>
+      <c r="P8" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q8">
+        <v>100000000</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8" t="b">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <v>-90.296190999999993</v>
+      </c>
+      <c r="U8">
+        <v>43.223405999999997</v>
+      </c>
+      <c r="V8">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9">
+        <v>100000000</v>
+      </c>
+      <c r="F9">
+        <v>1000</v>
+      </c>
+      <c r="G9">
+        <v>700</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="3"/>
+        <v>4960</v>
+      </c>
+      <c r="J9">
+        <v>2</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
+      <c r="L9">
+        <v>2000</v>
+      </c>
+      <c r="M9">
+        <v>2010</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="4"/>
+        <v>558000</v>
+      </c>
+      <c r="O9" t="s">
+        <v>67</v>
+      </c>
+      <c r="P9" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q9">
+        <v>100000000</v>
+      </c>
+      <c r="R9">
+        <v>1</v>
+      </c>
+      <c r="S9" t="b">
+        <v>1</v>
+      </c>
+      <c r="T9">
+        <v>-90.295739999999995</v>
+      </c>
+      <c r="U9">
+        <v>43.223359000000002</v>
+      </c>
+      <c r="V9">
+        <v>700</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -594,30 +1253,30 @@
     <col min="14" max="14" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G1" t="s">
-        <v>66</v>
-      </c>
       <c r="H1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -638,53 +1297,43 @@
         <v>9</v>
       </c>
       <c r="O1" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="P1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Q1" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="R1" t="s">
-        <v>55</v>
-      </c>
-      <c r="S1" t="s">
-        <v>61</v>
-      </c>
-      <c r="T1" t="s">
-        <v>62</v>
-      </c>
-      <c r="U1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>60000</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2">
+        <f>-PMT(0.05/12,360,(M2-M2*0.1),0)</f>
+        <v>1482.7550049218294</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2">
-        <f>12*H2/0.25</f>
-        <v>119040</v>
-      </c>
-      <c r="E2">
-        <v>1000</v>
-      </c>
-      <c r="F2">
-        <v>700</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <f>2.48*K2</f>
-        <v>2480</v>
+      <c r="H2" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -693,694 +1342,90 @@
         <v>1</v>
       </c>
       <c r="K2">
-        <v>1000</v>
+        <v>1100</v>
       </c>
       <c r="L2">
         <v>1920</v>
       </c>
       <c r="M2">
-        <f>279*K2</f>
-        <v>279000</v>
+        <f>K2*279</f>
+        <v>306900</v>
       </c>
       <c r="N2" t="s">
-        <v>45</v>
-      </c>
-      <c r="O2" t="s">
-        <v>38</v>
+        <v>18</v>
+      </c>
+      <c r="O2" t="b">
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>30000</v>
+        <v>-90.296126999999998</v>
       </c>
       <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2" t="b">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>-90.294238000000007</v>
-      </c>
-      <c r="T2">
-        <v>43.224015000000001</v>
-      </c>
-      <c r="U2">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+        <v>43.224344000000002</v>
+      </c>
+      <c r="R2">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>1000000</v>
+      </c>
+      <c r="C3">
+        <v>100</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2">
+        <f t="shared" ref="F3:F9" si="0">-PMT(0.05/12,360,(M3-M3*0.1),0)</f>
+        <v>4043.8772861504435</v>
+      </c>
+      <c r="G3" t="s">
         <v>15</v>
       </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D5" si="0">12*H3/0.25</f>
-        <v>178560</v>
-      </c>
-      <c r="E3">
-        <v>1000</v>
-      </c>
-      <c r="F3">
-        <v>700</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <f t="shared" ref="H3:H9" si="1">2.48*K3</f>
-        <v>3720</v>
+      <c r="H3" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="I3">
+        <v>4</v>
+      </c>
+      <c r="J3">
         <v>3</v>
       </c>
-      <c r="J3">
-        <v>2</v>
-      </c>
       <c r="K3">
-        <v>1500</v>
+        <v>3000</v>
       </c>
       <c r="L3">
         <v>1920</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M9" si="2">279*K3</f>
-        <v>418500</v>
+        <f t="shared" ref="M3:M5" si="1">K3*279</f>
+        <v>837000</v>
       </c>
       <c r="N3" t="s">
-        <v>44</v>
-      </c>
-      <c r="O3" t="s">
-        <v>39</v>
+        <v>45</v>
+      </c>
+      <c r="O3" t="b">
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>30000</v>
+        <v>-90.295697000000004</v>
       </c>
       <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3" t="b">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>-90.293766000000005</v>
-      </c>
-      <c r="T3">
-        <v>43.224062000000004</v>
-      </c>
-      <c r="U3">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
-        <v>59520</v>
-      </c>
-      <c r="E4">
-        <v>1000</v>
-      </c>
-      <c r="F4">
-        <v>700</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <f t="shared" si="1"/>
-        <v>1240</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <v>500</v>
-      </c>
-      <c r="L4">
-        <v>1960</v>
-      </c>
-      <c r="M4">
-        <f t="shared" si="2"/>
-        <v>139500</v>
-      </c>
-      <c r="N4" t="s">
-        <v>46</v>
-      </c>
-      <c r="O4" t="s">
-        <v>40</v>
-      </c>
-      <c r="P4">
-        <v>30000</v>
-      </c>
-      <c r="Q4">
-        <v>1</v>
-      </c>
-      <c r="R4" t="b">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>-90.293294000000003</v>
-      </c>
-      <c r="T4">
-        <v>43.224125000000001</v>
-      </c>
-      <c r="U4">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>238080</v>
-      </c>
-      <c r="E5">
-        <v>1000</v>
-      </c>
-      <c r="F5">
-        <v>700</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="1"/>
-        <v>4960</v>
-      </c>
-      <c r="I5">
-        <v>2</v>
-      </c>
-      <c r="J5">
-        <v>2</v>
-      </c>
-      <c r="K5">
-        <v>2000</v>
-      </c>
-      <c r="L5">
-        <v>2010</v>
-      </c>
-      <c r="M5">
-        <f t="shared" si="2"/>
-        <v>558000</v>
-      </c>
-      <c r="N5" t="s">
-        <v>18</v>
-      </c>
-      <c r="O5" t="s">
-        <v>41</v>
-      </c>
-      <c r="P5">
-        <v>30000</v>
-      </c>
-      <c r="Q5">
-        <v>1</v>
-      </c>
-      <c r="R5" t="b">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>-90.293058000000002</v>
-      </c>
-      <c r="T5">
-        <v>43.223936999999999</v>
-      </c>
-      <c r="U5">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6">
-        <v>100000000</v>
-      </c>
-      <c r="E6">
-        <v>1000</v>
-      </c>
-      <c r="F6">
-        <v>700</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <f>2.48*K6</f>
-        <v>2480</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-      <c r="K6">
-        <v>1000</v>
-      </c>
-      <c r="L6">
-        <v>1920</v>
-      </c>
-      <c r="M6">
-        <f>279*K6</f>
-        <v>279000</v>
-      </c>
-      <c r="N6" t="s">
-        <v>67</v>
-      </c>
-      <c r="O6" t="s">
-        <v>56</v>
-      </c>
-      <c r="P6">
-        <v>100000000</v>
-      </c>
-      <c r="Q6">
-        <v>1</v>
-      </c>
-      <c r="R6" t="b">
-        <v>1</v>
-      </c>
-      <c r="S6">
-        <v>-90.293080000000003</v>
-      </c>
-      <c r="T6">
-        <v>43.223671000000003</v>
-      </c>
-      <c r="U6">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7">
-        <v>100000000</v>
-      </c>
-      <c r="E7">
-        <v>1000</v>
-      </c>
-      <c r="F7">
-        <v>700</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <f t="shared" ref="H7:H9" si="3">2.48*K7</f>
-        <v>3720</v>
-      </c>
-      <c r="I7">
-        <v>3</v>
-      </c>
-      <c r="J7">
-        <v>2</v>
-      </c>
-      <c r="K7">
-        <v>1500</v>
-      </c>
-      <c r="L7">
-        <v>1920</v>
-      </c>
-      <c r="M7">
-        <f t="shared" ref="M7:M9" si="4">279*K7</f>
-        <v>418500</v>
-      </c>
-      <c r="N7" t="s">
-        <v>67</v>
-      </c>
-      <c r="O7" t="s">
-        <v>57</v>
-      </c>
-      <c r="P7">
-        <v>100000000</v>
-      </c>
-      <c r="Q7">
-        <v>1</v>
-      </c>
-      <c r="R7" t="b">
-        <v>1</v>
-      </c>
-      <c r="S7">
-        <v>-90.292736000000005</v>
-      </c>
-      <c r="T7">
-        <v>43.223545999999999</v>
-      </c>
-      <c r="U7">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8">
-        <v>100000000</v>
-      </c>
-      <c r="E8">
-        <v>1000</v>
-      </c>
-      <c r="F8">
-        <v>700</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="3"/>
-        <v>1240</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-      <c r="K8">
-        <v>500</v>
-      </c>
-      <c r="L8">
-        <v>1960</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="4"/>
-        <v>139500</v>
-      </c>
-      <c r="N8" t="s">
-        <v>67</v>
-      </c>
-      <c r="O8" t="s">
-        <v>58</v>
-      </c>
-      <c r="P8">
-        <v>100000000</v>
-      </c>
-      <c r="Q8">
-        <v>1</v>
-      </c>
-      <c r="R8" t="b">
-        <v>1</v>
-      </c>
-      <c r="S8">
-        <v>-90.296190999999993</v>
-      </c>
-      <c r="T8">
-        <v>43.223405999999997</v>
-      </c>
-      <c r="U8">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9">
-        <v>100000000</v>
-      </c>
-      <c r="E9">
-        <v>1000</v>
-      </c>
-      <c r="F9">
-        <v>700</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="3"/>
-        <v>4960</v>
-      </c>
-      <c r="I9">
-        <v>2</v>
-      </c>
-      <c r="J9">
-        <v>2</v>
-      </c>
-      <c r="K9">
-        <v>2000</v>
-      </c>
-      <c r="L9">
-        <v>2010</v>
-      </c>
-      <c r="M9">
-        <f t="shared" si="4"/>
-        <v>558000</v>
-      </c>
-      <c r="N9" t="s">
-        <v>67</v>
-      </c>
-      <c r="O9" t="s">
-        <v>59</v>
-      </c>
-      <c r="P9">
-        <v>100000000</v>
-      </c>
-      <c r="Q9">
-        <v>1</v>
-      </c>
-      <c r="R9" t="b">
-        <v>1</v>
-      </c>
-      <c r="S9">
-        <v>-90.295739999999995</v>
-      </c>
-      <c r="T9">
-        <v>43.223359000000002</v>
-      </c>
-      <c r="U9">
-        <v>700</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="13" max="13" width="16.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" t="s">
-        <v>55</v>
-      </c>
-      <c r="O1" t="s">
-        <v>61</v>
-      </c>
-      <c r="P1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2">
-        <v>60000</v>
-      </c>
-      <c r="C2">
-        <v>100</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="2">
-        <f>-PMT(0.05/12,360,(L2-L2*0.1),0)</f>
-        <v>1482.7550049218294</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1100</v>
-      </c>
-      <c r="K2">
-        <v>1920</v>
-      </c>
-      <c r="L2">
-        <f>J2*279</f>
-        <v>306900</v>
-      </c>
-      <c r="M2" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" t="b">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>-90.296126999999998</v>
-      </c>
-      <c r="P2">
-        <v>43.224344000000002</v>
-      </c>
-      <c r="Q2">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3">
-        <v>1000000</v>
-      </c>
-      <c r="C3">
-        <v>100</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="2">
-        <f t="shared" ref="F3:F9" si="0">-PMT(0.05/12,360,(L3-L3*0.1),0)</f>
-        <v>4043.8772861504435</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3">
-        <v>4</v>
-      </c>
-      <c r="I3">
-        <v>3</v>
-      </c>
-      <c r="J3">
-        <v>3000</v>
-      </c>
-      <c r="K3">
-        <v>1920</v>
-      </c>
-      <c r="L3">
-        <f t="shared" ref="L3:L5" si="1">J3*279</f>
-        <v>837000</v>
-      </c>
-      <c r="M3" t="s">
-        <v>45</v>
-      </c>
-      <c r="N3" t="b">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>-90.295697000000004</v>
-      </c>
-      <c r="P3">
         <v>43.224218999999998</v>
       </c>
-      <c r="Q3">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R3">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1403,39 +1448,42 @@
       <c r="G4" t="s">
         <v>15</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I4">
         <v>2</v>
       </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
       <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
         <v>750</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>1960</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <f t="shared" si="1"/>
         <v>209250</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>46</v>
       </c>
-      <c r="N4" t="b">
-        <v>0</v>
-      </c>
-      <c r="O4">
+      <c r="O4" t="b">
+        <v>0</v>
+      </c>
+      <c r="P4">
         <v>-90.296706</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>43.223984000000002</v>
       </c>
-      <c r="Q4">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R4">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1458,39 +1506,42 @@
       <c r="G5" t="s">
         <v>15</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I5">
         <v>3</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>2</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>2000</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>2010</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <f t="shared" si="1"/>
         <v>558000</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>44</v>
       </c>
-      <c r="N5" t="b">
-        <v>0</v>
-      </c>
-      <c r="O5">
+      <c r="O5" t="b">
+        <v>0</v>
+      </c>
+      <c r="P5">
         <v>-90.296642000000006</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>43.223750000000003</v>
       </c>
-      <c r="Q5">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R5">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -1513,38 +1564,41 @@
       <c r="G6" t="s">
         <v>12</v>
       </c>
-      <c r="H6">
-        <v>1</v>
+      <c r="H6" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="I6">
         <v>1</v>
       </c>
       <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
         <v>1100</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>1920</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>300000</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>67</v>
       </c>
-      <c r="N6" t="b">
-        <v>1</v>
-      </c>
-      <c r="O6">
+      <c r="O6" t="b">
+        <v>1</v>
+      </c>
+      <c r="P6">
         <v>-90.295053999999993</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>43.224375000000002</v>
       </c>
-      <c r="Q6">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R6">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>48</v>
       </c>
@@ -1567,38 +1621,41 @@
       <c r="G7" t="s">
         <v>15</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I7">
         <v>4</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>3</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>3000</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>1920</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>800000</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>67</v>
       </c>
-      <c r="N7" t="b">
-        <v>1</v>
-      </c>
-      <c r="O7">
+      <c r="O7" t="b">
+        <v>1</v>
+      </c>
+      <c r="P7">
         <v>-90.294539</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>43.224390999999997</v>
       </c>
-      <c r="Q7">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R7">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -1621,38 +1678,41 @@
       <c r="G8" t="s">
         <v>15</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I8">
         <v>2</v>
       </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
       <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
         <v>750</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>1960</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>300000</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>67</v>
       </c>
-      <c r="N8" t="b">
-        <v>1</v>
-      </c>
-      <c r="O8">
+      <c r="O8" t="b">
+        <v>1</v>
+      </c>
+      <c r="P8">
         <v>-90.295225000000002</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>43.223953000000002</v>
       </c>
-      <c r="Q8">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R8">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -1675,34 +1735,37 @@
       <c r="G9" t="s">
         <v>15</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I9">
         <v>3</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>2</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>2000</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>2010</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>500000</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>67</v>
       </c>
-      <c r="N9" t="b">
-        <v>1</v>
-      </c>
-      <c r="O9">
+      <c r="O9" t="b">
+        <v>1</v>
+      </c>
+      <c r="P9">
         <v>-90.295225000000002</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>43.223717999999998</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>700</v>
       </c>
     </row>

</xml_diff>